<commit_message>
Consolidate files; detrend excess demand
</commit_message>
<xml_diff>
--- a/Replication Package/Code and Data/(1) Data/Public Data/Regression_Data.xlsx
+++ b/Replication Package/Code and Data/(1) Data/Public Data/Regression_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnathansun/Documents/ec1499/Replication Package/Code and Data/(1) Data/Public Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8AB7CF-FF96-2C43-B455-1BE31239B42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC835D86-DA23-E448-BA17-F7CF345E6B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="25080" windowHeight="18980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25080" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="367">
   <si>
     <t>Date</t>
   </si>
@@ -1135,12 +1135,6 @@
   </si>
   <si>
     <t>Capacity Utilization: Total Index, Percent, Seasonally Adjusted</t>
-  </si>
-  <si>
-    <t>TCU_DETRENDED</t>
-  </si>
-  <si>
-    <t>Capacity Utilization: Total Index, Percent, Seasonally Adjusted minus 10Y rolling average</t>
   </si>
 </sst>
 </file>
@@ -1532,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S309"/>
+  <dimension ref="A1:R309"/>
   <sheetViews>
-    <sheetView topLeftCell="B133" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1548,7 +1542,7 @@
     <col min="19" max="19" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1603,11 +1597,8 @@
       <c r="R1" t="s">
         <v>362</v>
       </c>
-      <c r="S1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1648,7 +1639,7 @@
         <v>274.03395189999998</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1689,7 +1680,7 @@
         <v>276.282610699999</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1730,7 +1721,7 @@
         <v>278.32913769999999</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1771,7 +1762,7 @@
         <v>282.05581599999999</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -1812,7 +1803,7 @@
         <v>284.9172681</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1853,7 +1844,7 @@
         <v>289.75882200000001</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1894,7 +1885,7 @@
         <v>299.9053002</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1935,7 +1926,7 @@
         <v>309.42480599999999</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -1976,7 +1967,7 @@
         <v>274.03395189999998</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2017,7 +2008,7 @@
         <v>276.282610699999</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -2058,7 +2049,7 @@
         <v>278.32913769999999</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -2099,7 +2090,7 @@
         <v>282.05581599999999</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -2140,7 +2131,7 @@
         <v>284.9172681</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -2181,7 +2172,7 @@
         <v>289.75882200000001</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -4939,7 +4930,7 @@
         <v>783.08203000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>126</v>
       </c>
@@ -4983,7 +4974,7 @@
         <v>798.24810319999995</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>127</v>
       </c>
@@ -5029,11 +5020,8 @@
       <c r="R82">
         <v>810.46956990000001</v>
       </c>
-      <c r="S82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>128</v>
       </c>
@@ -5079,11 +5067,8 @@
       <c r="R83">
         <v>823.78636189999997</v>
       </c>
-      <c r="S83">
-        <v>-0.77048333333333097</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>129</v>
       </c>
@@ -5129,11 +5114,8 @@
       <c r="R84">
         <v>841.14886569999999</v>
       </c>
-      <c r="S84">
-        <v>-0.89063333333332595</v>
-      </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>130</v>
       </c>
@@ -5179,11 +5161,8 @@
       <c r="R85">
         <v>860.33641979999902</v>
       </c>
-      <c r="S85">
-        <v>0.18962499999999199</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>131</v>
       </c>
@@ -5229,11 +5208,8 @@
       <c r="R86">
         <v>879.90035479999995</v>
       </c>
-      <c r="S86">
-        <v>0.27361999999999398</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>132</v>
       </c>
@@ -5279,11 +5255,8 @@
       <c r="R87">
         <v>899.09676979999995</v>
       </c>
-      <c r="S87">
-        <v>0.34334999999999999</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>133</v>
       </c>
@@ -5329,11 +5302,8 @@
       <c r="R88">
         <v>918.06164620000004</v>
       </c>
-      <c r="S88">
-        <v>6.7142857143664904E-4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>134</v>
       </c>
@@ -5379,11 +5349,8 @@
       <c r="R89">
         <v>941.34386359999996</v>
       </c>
-      <c r="S89">
-        <v>0.27011666666665202</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>135</v>
       </c>
@@ -5429,11 +5396,8 @@
       <c r="R90">
         <v>961.17875230000004</v>
       </c>
-      <c r="S90">
-        <v>0.87696296296296306</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>136</v>
       </c>
@@ -5479,11 +5443,8 @@
       <c r="R91">
         <v>983.3084523</v>
       </c>
-      <c r="S91">
-        <v>0.28811666666668101</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>137</v>
       </c>
@@ -5529,11 +5490,8 @@
       <c r="R92">
         <v>1006.55299</v>
       </c>
-      <c r="S92">
-        <v>0.36916666666667097</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>138</v>
       </c>
@@ -5579,11 +5537,8 @@
       <c r="R93">
         <v>1028.7076999999999</v>
       </c>
-      <c r="S93">
-        <v>-0.99757777777777701</v>
-      </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>139</v>
       </c>
@@ -5635,11 +5590,8 @@
       <c r="R94">
         <v>1052.2456279999999</v>
       </c>
-      <c r="S94">
-        <v>-3.6157333333333299</v>
-      </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>140</v>
       </c>
@@ -5691,11 +5643,8 @@
       <c r="R95">
         <v>1075.632435</v>
       </c>
-      <c r="S95">
-        <v>-4.4966999999999997</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>141</v>
       </c>
@@ -5747,11 +5696,8 @@
       <c r="R96">
         <v>1092.998726</v>
       </c>
-      <c r="S96">
-        <v>-5.1729066666666599</v>
-      </c>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>142</v>
       </c>
@@ -5803,11 +5749,8 @@
       <c r="R97">
         <v>1115.9525349999999</v>
       </c>
-      <c r="S97">
-        <v>-7.1719749999999998</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -5859,11 +5802,8 @@
       <c r="R98">
         <v>1141.9851570000001</v>
       </c>
-      <c r="S98">
-        <v>-5.95</v>
-      </c>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>144</v>
       </c>
@@ -5915,11 +5855,8 @@
       <c r="R99">
         <v>1166.644875</v>
       </c>
-      <c r="S99">
-        <v>-5.5124074074073999</v>
-      </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>145</v>
       </c>
@@ -5971,11 +5908,8 @@
       <c r="R100">
         <v>1188.677003</v>
       </c>
-      <c r="S100">
-        <v>-5.55682807017544</v>
-      </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>146</v>
       </c>
@@ -6027,11 +5961,8 @@
       <c r="R101">
         <v>1208.845086</v>
       </c>
-      <c r="S101">
-        <v>-4.10846</v>
-      </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>147</v>
       </c>
@@ -6083,11 +6014,8 @@
       <c r="R102">
         <v>1237.3963349999999</v>
       </c>
-      <c r="S102">
-        <v>-1.24059682539682</v>
-      </c>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>148</v>
       </c>
@@ -6139,11 +6067,8 @@
       <c r="R103">
         <v>1254.8895680000001</v>
       </c>
-      <c r="S103">
-        <v>-0.268574242424236</v>
-      </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>149</v>
       </c>
@@ -6195,11 +6120,8 @@
       <c r="R104">
         <v>1276.5064890000001</v>
       </c>
-      <c r="S104">
-        <v>0.123575362318831</v>
-      </c>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>150</v>
       </c>
@@ -6251,11 +6173,8 @@
       <c r="R105">
         <v>1302.520021</v>
       </c>
-      <c r="S105">
-        <v>2.1988722222222199</v>
-      </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>151</v>
       </c>
@@ -6307,11 +6226,8 @@
       <c r="R106">
         <v>1327.7102190000001</v>
       </c>
-      <c r="S106">
-        <v>3.6723573333333199</v>
-      </c>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>152</v>
       </c>
@@ -6363,11 +6279,8 @@
       <c r="R107">
         <v>1359.1456390000001</v>
       </c>
-      <c r="S107">
-        <v>3.3940935897436</v>
-      </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>153</v>
       </c>
@@ -6419,11 +6332,8 @@
       <c r="R108">
         <v>1397.1871329999999</v>
       </c>
-      <c r="S108">
-        <v>3.1052283950617201</v>
-      </c>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>154</v>
       </c>
@@ -6475,11 +6385,8 @@
       <c r="R109">
         <v>1437.3338099999901</v>
       </c>
-      <c r="S109">
-        <v>3.4495345238095299</v>
-      </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>155</v>
       </c>
@@ -6531,11 +6438,8 @@
       <c r="R110">
         <v>1477.099463</v>
       </c>
-      <c r="S110">
-        <v>1.77320574712643</v>
-      </c>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>156</v>
       </c>
@@ -6587,11 +6491,8 @@
       <c r="R111">
         <v>1525.0964240000001</v>
       </c>
-      <c r="S111">
-        <v>1.0851211111111201</v>
-      </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>157</v>
       </c>
@@ -6643,11 +6544,8 @@
       <c r="R112">
         <v>1582.9788920000001</v>
       </c>
-      <c r="S112">
-        <v>0.17085913978495099</v>
-      </c>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>158</v>
       </c>
@@ -6699,11 +6597,8 @@
       <c r="R113">
         <v>1643.0582609999999</v>
       </c>
-      <c r="S113">
-        <v>-3.59084062499999</v>
-      </c>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>159</v>
       </c>
@@ -6755,11 +6650,8 @@
       <c r="R114">
         <v>1693.87701499999</v>
       </c>
-      <c r="S114">
-        <v>-9.1500676767676694</v>
-      </c>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>160</v>
       </c>
@@ -6811,11 +6703,8 @@
       <c r="R115">
         <v>1732.6305789999999</v>
       </c>
-      <c r="S115">
-        <v>-10.1805009803921</v>
-      </c>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>161</v>
       </c>
@@ -6867,11 +6756,8 @@
       <c r="R116">
         <v>1776.8473059999999</v>
       </c>
-      <c r="S116">
-        <v>-8.4637019047618995</v>
-      </c>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>162</v>
       </c>
@@ -6923,11 +6809,8 @@
       <c r="R117">
         <v>1820.4053819999999</v>
       </c>
-      <c r="S117">
-        <v>-7.0151685185185197</v>
-      </c>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>163</v>
       </c>
@@ -6979,11 +6862,8 @@
       <c r="R118">
         <v>1853.490335</v>
       </c>
-      <c r="S118">
-        <v>-5.0105207207207201</v>
-      </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>164</v>
       </c>
@@ -7035,11 +6915,8 @@
       <c r="R119">
         <v>1886.1097949999901</v>
       </c>
-      <c r="S119">
-        <v>-4.3917903508771801</v>
-      </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>165</v>
       </c>
@@ -7091,11 +6968,8 @@
       <c r="R120">
         <v>1925.04763</v>
       </c>
-      <c r="S120">
-        <v>-3.76445897435898</v>
-      </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>166</v>
       </c>
@@ -7147,11 +7021,8 @@
       <c r="R121">
         <v>1974.4854439999999</v>
       </c>
-      <c r="S121">
-        <v>-2.8169949999999999</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>167</v>
       </c>
@@ -7203,11 +7074,8 @@
       <c r="R122">
         <v>2021.8984329999901</v>
       </c>
-      <c r="S122">
-        <v>-1.63920833333334</v>
-      </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>168</v>
       </c>
@@ -7259,11 +7127,8 @@
       <c r="R123">
         <v>2067.0156699999998</v>
       </c>
-      <c r="S123">
-        <v>0.36060833333333098</v>
-      </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>169</v>
       </c>
@@ -7315,11 +7180,8 @@
       <c r="R124">
         <v>2109.323249</v>
       </c>
-      <c r="S124">
-        <v>0.66306583333333402</v>
-      </c>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>170</v>
       </c>
@@ -7371,11 +7233,8 @@
       <c r="R125">
         <v>2172.916725</v>
       </c>
-      <c r="S125">
-        <v>0.57845083333333402</v>
-      </c>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>171</v>
       </c>
@@ -7427,11 +7286,8 @@
       <c r="R126">
         <v>2223.2557160000001</v>
       </c>
-      <c r="S126">
-        <v>-0.26296916666667802</v>
-      </c>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>172</v>
       </c>
@@ -7483,11 +7339,8 @@
       <c r="R127">
         <v>2285.131433</v>
       </c>
-      <c r="S127">
-        <v>2.43929166666666</v>
-      </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>173</v>
       </c>
@@ -7539,11 +7392,8 @@
       <c r="R128">
         <v>2344.2615839999999</v>
       </c>
-      <c r="S128">
-        <v>2.51873999999999</v>
-      </c>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>174</v>
       </c>
@@ -7595,11 +7445,8 @@
       <c r="R129">
         <v>2413.2887460000002</v>
       </c>
-      <c r="S129">
-        <v>3.33784666666666</v>
-      </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>175</v>
       </c>
@@ -7651,11 +7498,8 @@
       <c r="R130">
         <v>2479.5954430000002</v>
       </c>
-      <c r="S130">
-        <v>3.10654083333334</v>
-      </c>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>176</v>
       </c>
@@ -7707,11 +7551,8 @@
       <c r="R131">
         <v>2562.373681</v>
       </c>
-      <c r="S131">
-        <v>2.3094225000000099</v>
-      </c>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>177</v>
       </c>
@@ -7763,11 +7604,8 @@
       <c r="R132">
         <v>2639.8152439999999</v>
       </c>
-      <c r="S132">
-        <v>1.5256766666666799</v>
-      </c>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>178</v>
       </c>
@@ -7819,11 +7657,8 @@
       <c r="R133">
         <v>2708.8784639999999</v>
       </c>
-      <c r="S133">
-        <v>1.37828999999999</v>
-      </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>179</v>
       </c>
@@ -7875,11 +7710,8 @@
       <c r="R134">
         <v>2784.0217789999901</v>
       </c>
-      <c r="S134">
-        <v>1.22371916666665</v>
-      </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>180</v>
       </c>
@@ -7931,11 +7763,8 @@
       <c r="R135">
         <v>2866.5326500000001</v>
       </c>
-      <c r="S135">
-        <v>-2.7384550000000001</v>
-      </c>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>181</v>
       </c>
@@ -7987,11 +7816,8 @@
       <c r="R136">
         <v>2944.5695179999998</v>
       </c>
-      <c r="S136">
-        <v>-4.4319383333333304</v>
-      </c>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>182</v>
       </c>
@@ -8043,11 +7869,8 @@
       <c r="R137">
         <v>3036.4104010000001</v>
       </c>
-      <c r="S137">
-        <v>-1.9756466666666599</v>
-      </c>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>183</v>
       </c>
@@ -8099,11 +7922,8 @@
       <c r="R138">
         <v>3126.3115320000002</v>
       </c>
-      <c r="S138">
-        <v>-2.37386916666666</v>
-      </c>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>184</v>
       </c>
@@ -8155,11 +7975,8 @@
       <c r="R139">
         <v>3208.3339620000002</v>
       </c>
-      <c r="S139">
-        <v>-2.74078166666667</v>
-      </c>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>185</v>
       </c>
@@ -8211,11 +8028,8 @@
       <c r="R140">
         <v>3290.6037350000001</v>
       </c>
-      <c r="S140">
-        <v>-2.6190408333333099</v>
-      </c>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>186</v>
       </c>
@@ -8267,11 +8081,8 @@
       <c r="R141">
         <v>3371.1634009999998</v>
       </c>
-      <c r="S141">
-        <v>-4.9268233333333296</v>
-      </c>
-    </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>187</v>
       </c>
@@ -8323,11 +8134,8 @@
       <c r="R142">
         <v>3442.7524869999902</v>
       </c>
-      <c r="S142">
-        <v>-6.8240274999999997</v>
-      </c>
-    </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>188</v>
       </c>
@@ -8379,11 +8187,8 @@
       <c r="R143">
         <v>3513.7869289999999</v>
       </c>
-      <c r="S143">
-        <v>-7.9142258333333402</v>
-      </c>
-    </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>189</v>
       </c>
@@ -8435,11 +8240,8 @@
       <c r="R144">
         <v>3590.9186100000002</v>
       </c>
-      <c r="S144">
-        <v>-8.9808808333333499</v>
-      </c>
-    </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>190</v>
       </c>
@@ -8491,11 +8293,8 @@
       <c r="R145">
         <v>3656.536525</v>
       </c>
-      <c r="S145">
-        <v>-10.172499166666601</v>
-      </c>
-    </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>191</v>
       </c>
@@ -8547,11 +8346,8 @@
       <c r="R146">
         <v>3712.5106619999901</v>
       </c>
-      <c r="S146">
-        <v>-9.0769183333333299</v>
-      </c>
-    </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>192</v>
       </c>
@@ -8603,11 +8399,8 @@
       <c r="R147">
         <v>3769.3899219999998</v>
       </c>
-      <c r="S147">
-        <v>-7.1706174999999996</v>
-      </c>
-    </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>193</v>
       </c>
@@ -8659,11 +8452,8 @@
       <c r="R148">
         <v>3840.055061</v>
       </c>
-      <c r="S148">
-        <v>-4.44016583333332</v>
-      </c>
-    </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>194</v>
       </c>
@@ -8715,11 +8505,8 @@
       <c r="R149">
         <v>3901.1061799999902</v>
       </c>
-      <c r="S149">
-        <v>-2.3465525</v>
-      </c>
-    </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>195</v>
       </c>
@@ -8771,11 +8558,8 @@
       <c r="R150">
         <v>3974.2638459999998</v>
       </c>
-      <c r="S150">
-        <v>-0.13724333333334399</v>
-      </c>
-    </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>196</v>
       </c>
@@ -8827,11 +8611,8 @@
       <c r="R151">
         <v>4043.3373579999902</v>
       </c>
-      <c r="S151">
-        <v>0.85581750000000001</v>
-      </c>
-    </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>197</v>
       </c>
@@ -8883,11 +8664,8 @@
       <c r="R152">
         <v>4115.627759</v>
       </c>
-      <c r="S152">
-        <v>1.0203941666666601</v>
-      </c>
-    </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>198</v>
       </c>
@@ -8939,11 +8717,8 @@
       <c r="R153">
         <v>4183.5817029999998</v>
       </c>
-      <c r="S153">
-        <v>0.53422916666666198</v>
-      </c>
-    </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>199</v>
       </c>
@@ -8995,11 +8770,8 @@
       <c r="R154">
         <v>4262.6752850000003</v>
       </c>
-      <c r="S154">
-        <v>9.8650833333323307E-2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>200</v>
       </c>
@@ -9051,11 +8823,8 @@
       <c r="R155">
         <v>4328.1549059999998</v>
       </c>
-      <c r="S155">
-        <v>-0.59628416666664896</v>
-      </c>
-    </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>201</v>
       </c>
@@ -9107,11 +8876,8 @@
       <c r="R156">
         <v>4392.479155</v>
       </c>
-      <c r="S156">
-        <v>-1.3459975000000099</v>
-      </c>
-    </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>202</v>
       </c>
@@ -9163,11 +8929,8 @@
       <c r="R157">
         <v>4455.1133170000003</v>
       </c>
-      <c r="S157">
-        <v>-1.4070425</v>
-      </c>
-    </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>203</v>
       </c>
@@ -9219,11 +8982,8 @@
       <c r="R158">
         <v>4515.1490439999998</v>
       </c>
-      <c r="S158">
-        <v>-1.2851033333333299</v>
-      </c>
-    </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>204</v>
       </c>
@@ -9275,11 +9035,8 @@
       <c r="R159">
         <v>4569.816417</v>
       </c>
-      <c r="S159">
-        <v>-1.9902658333333301</v>
-      </c>
-    </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>205</v>
       </c>
@@ -9331,11 +9088,8 @@
       <c r="R160">
         <v>4626.1940379999996</v>
       </c>
-      <c r="S160">
-        <v>-1.87504916666667</v>
-      </c>
-    </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>206</v>
       </c>
@@ -9387,11 +9141,8 @@
       <c r="R161">
         <v>4689.2588850000002</v>
       </c>
-      <c r="S161">
-        <v>-1.23339666666667</v>
-      </c>
-    </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>207</v>
       </c>
@@ -9443,11 +9194,8 @@
       <c r="R162">
         <v>4757.3731019999996</v>
       </c>
-      <c r="S162">
-        <v>-0.495587500000013</v>
-      </c>
-    </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>208</v>
       </c>
@@ -9499,11 +9247,8 @@
       <c r="R163">
         <v>4828.5929640000004</v>
       </c>
-      <c r="S163">
-        <v>0.52839333333334004</v>
-      </c>
-    </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>209</v>
       </c>
@@ -9555,11 +9300,8 @@
       <c r="R164">
         <v>4903.6704259999997</v>
       </c>
-      <c r="S164">
-        <v>1.6231324999999901</v>
-      </c>
-    </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>210</v>
       </c>
@@ -9611,11 +9353,8 @@
       <c r="R165">
         <v>4981.7766700000002</v>
       </c>
-      <c r="S165">
-        <v>3.17699166666665</v>
-      </c>
-    </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>211</v>
       </c>
@@ -9667,11 +9406,8 @@
       <c r="R166">
         <v>5060.2075560000003</v>
       </c>
-      <c r="S166">
-        <v>3.6767933333333298</v>
-      </c>
-    </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>212</v>
       </c>
@@ -9723,11 +9459,8 @@
       <c r="R167">
         <v>5149.3756999999996</v>
       </c>
-      <c r="S167">
-        <v>4.3078399999999899</v>
-      </c>
-    </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>213</v>
       </c>
@@ -9779,11 +9512,8 @@
       <c r="R168">
         <v>5251.528894</v>
       </c>
-      <c r="S168">
-        <v>4.5532658333333398</v>
-      </c>
-    </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>214</v>
       </c>
@@ -9835,11 +9565,8 @@
       <c r="R169">
         <v>5338.2009420000004</v>
       </c>
-      <c r="S169">
-        <v>5.0235366666666703</v>
-      </c>
-    </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>215</v>
       </c>
@@ -9891,11 +9618,8 @@
       <c r="R170">
         <v>5435.697811</v>
       </c>
-      <c r="S170">
-        <v>5.1605549999999996</v>
-      </c>
-    </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>216</v>
       </c>
@@ -9947,11 +9671,8 @@
       <c r="R171">
         <v>5535.86913</v>
       </c>
-      <c r="S171">
-        <v>4.4437308333333396</v>
-      </c>
-    </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>217</v>
       </c>
@@ -10003,11 +9724,8 @@
       <c r="R172">
         <v>5618.9537499999997</v>
       </c>
-      <c r="S172">
-        <v>3.4258233333333101</v>
-      </c>
-    </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>218</v>
       </c>
@@ -10059,11 +9777,8 @@
       <c r="R173">
         <v>5701.639795</v>
       </c>
-      <c r="S173">
-        <v>3.1964208333333302</v>
-      </c>
-    </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>219</v>
       </c>
@@ -10115,11 +9830,8 @@
       <c r="R174">
         <v>5805.9271710000003</v>
       </c>
-      <c r="S174">
-        <v>3.2527041666666698</v>
-      </c>
-    </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>220</v>
       </c>
@@ -10171,11 +9883,8 @@
       <c r="R175">
         <v>5913.4797399999998</v>
       </c>
-      <c r="S175">
-        <v>3.2102483333333298</v>
-      </c>
-    </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>221</v>
       </c>
@@ -10227,11 +9936,8 @@
       <c r="R176">
         <v>6006.0104849999998</v>
       </c>
-      <c r="S176">
-        <v>2.9655900000000002</v>
-      </c>
-    </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>222</v>
       </c>
@@ -10283,11 +9989,8 @@
       <c r="R177">
         <v>6091.7236670000002</v>
       </c>
-      <c r="S177">
-        <v>1.3320308333333299</v>
-      </c>
-    </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>223</v>
       </c>
@@ -10339,11 +10042,8 @@
       <c r="R178">
         <v>6191.9116809999996</v>
       </c>
-      <c r="S178">
-        <v>-0.444068333333348</v>
-      </c>
-    </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>224</v>
       </c>
@@ -10395,11 +10095,8 @@
       <c r="R179">
         <v>6277.1077580000001</v>
       </c>
-      <c r="S179">
-        <v>-0.21510166666665401</v>
-      </c>
-    </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>225</v>
       </c>
@@ -10451,11 +10148,8 @@
       <c r="R180">
         <v>6365.4781419999999</v>
       </c>
-      <c r="S180">
-        <v>0.67291500000000304</v>
-      </c>
-    </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>226</v>
       </c>
@@ -10507,11 +10201,8 @@
       <c r="R181">
         <v>6442.9497009999995</v>
       </c>
-      <c r="S181">
-        <v>0.47854833333332097</v>
-      </c>
-    </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>227</v>
       </c>
@@ -10563,11 +10254,8 @@
       <c r="R182">
         <v>6506.7752700000001</v>
       </c>
-      <c r="S182">
-        <v>-0.16788833333335099</v>
-      </c>
-    </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>228</v>
       </c>
@@ -10619,11 +10307,8 @@
       <c r="R183">
         <v>6586.491822</v>
       </c>
-      <c r="S183">
-        <v>0.59363749999999904</v>
-      </c>
-    </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>229</v>
       </c>
@@ -10675,11 +10360,8 @@
       <c r="R184">
         <v>6660.1796020000002</v>
       </c>
-      <c r="S184">
-        <v>0.49676999999999699</v>
-      </c>
-    </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>230</v>
       </c>
@@ -10731,11 +10413,8 @@
       <c r="R185">
         <v>6748.6188319999901</v>
       </c>
-      <c r="S185">
-        <v>0.580768333333324</v>
-      </c>
-    </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>231</v>
       </c>
@@ -10787,11 +10466,8 @@
       <c r="R186">
         <v>6829.8161959999998</v>
       </c>
-      <c r="S186">
-        <v>0.67437999999999898</v>
-      </c>
-    </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>232</v>
       </c>
@@ -10843,11 +10519,8 @@
       <c r="R187">
         <v>6915.2896099999998</v>
       </c>
-      <c r="S187">
-        <v>0.29727499999999901</v>
-      </c>
-    </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>233</v>
       </c>
@@ -10899,11 +10572,8 @@
       <c r="R188">
         <v>7002.2222299999903</v>
       </c>
-      <c r="S188">
-        <v>0.137911666666681</v>
-      </c>
-    </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>234</v>
       </c>
@@ -10955,11 +10625,8 @@
       <c r="R189">
         <v>7087.1289349999997</v>
       </c>
-      <c r="S189">
-        <v>0.86884750000000099</v>
-      </c>
-    </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>235</v>
       </c>
@@ -11011,11 +10678,8 @@
       <c r="R190">
         <v>7168.7985559999997</v>
       </c>
-      <c r="S190">
-        <v>1.25678666666667</v>
-      </c>
-    </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>236</v>
       </c>
@@ -11067,11 +10731,8 @@
       <c r="R191">
         <v>7251.8065569999899</v>
       </c>
-      <c r="S191">
-        <v>2.0274124999999898</v>
-      </c>
-    </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>237</v>
       </c>
@@ -11123,11 +10784,8 @@
       <c r="R192">
         <v>7343.2918540000001</v>
       </c>
-      <c r="S192">
-        <v>2.2570833333333402</v>
-      </c>
-    </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>238</v>
       </c>
@@ -11179,11 +10837,8 @@
       <c r="R193">
         <v>7434.1555840000001</v>
       </c>
-      <c r="S193">
-        <v>3.0288124999999999</v>
-      </c>
-    </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>239</v>
       </c>
@@ -11235,11 +10890,8 @@
       <c r="R194">
         <v>7526.2459250000002</v>
       </c>
-      <c r="S194">
-        <v>2.9491416666666601</v>
-      </c>
-    </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>240</v>
       </c>
@@ -11291,11 +10943,8 @@
       <c r="R195">
         <v>7615.5385819999901</v>
       </c>
-      <c r="S195">
-        <v>2.2369383333333199</v>
-      </c>
-    </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="196" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>241</v>
       </c>
@@ -11347,11 +10996,8 @@
       <c r="R196">
         <v>7706.9652889999998</v>
       </c>
-      <c r="S196">
-        <v>1.98530416666666</v>
-      </c>
-    </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="197" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>242</v>
       </c>
@@ -11403,11 +11049,8 @@
       <c r="R197">
         <v>7799.8132290000003</v>
       </c>
-      <c r="S197">
-        <v>1.5173808333333301</v>
-      </c>
-    </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>243</v>
       </c>
@@ -11459,11 +11102,8 @@
       <c r="R198">
         <v>7894.5567289999999</v>
       </c>
-      <c r="S198">
-        <v>0.861476666666675</v>
-      </c>
-    </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>244</v>
       </c>
@@ -11515,11 +11155,8 @@
       <c r="R199">
         <v>7988.2158040000004</v>
       </c>
-      <c r="S199">
-        <v>1.3489425000000199</v>
-      </c>
-    </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>245</v>
       </c>
@@ -11571,11 +11208,8 @@
       <c r="R200">
         <v>8079.9808890000004</v>
       </c>
-      <c r="S200">
-        <v>1.1529433333333099</v>
-      </c>
-    </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>246</v>
       </c>
@@ -11627,11 +11261,8 @@
       <c r="R201">
         <v>8193.5555000000004</v>
       </c>
-      <c r="S201">
-        <v>1.05867666666668</v>
-      </c>
-    </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>247</v>
       </c>
@@ -11683,11 +11314,8 @@
       <c r="R202">
         <v>8317.3596129999896</v>
       </c>
-      <c r="S202">
-        <v>1.3176650000000001</v>
-      </c>
-    </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>248</v>
       </c>
@@ -11739,11 +11367,8 @@
       <c r="R203">
         <v>8412.5565750000005</v>
       </c>
-      <c r="S203">
-        <v>1.1651975000000001</v>
-      </c>
-    </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>249</v>
       </c>
@@ -11795,11 +11420,8 @@
       <c r="R204">
         <v>8532.1647819999998</v>
       </c>
-      <c r="S204">
-        <v>1.6016366666666599</v>
-      </c>
-    </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>250</v>
       </c>
@@ -11851,11 +11473,8 @@
       <c r="R205">
         <v>8646.776124</v>
       </c>
-      <c r="S205">
-        <v>2.0569649999999902</v>
-      </c>
-    </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>251</v>
       </c>
@@ -11910,11 +11529,8 @@
       <c r="R206">
         <v>8748.0520730000007</v>
       </c>
-      <c r="S206">
-        <v>1.29724833333332</v>
-      </c>
-    </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>252</v>
       </c>
@@ -11969,11 +11585,8 @@
       <c r="R207">
         <v>8860.6284070000002</v>
       </c>
-      <c r="S207">
-        <v>0.259667499999991</v>
-      </c>
-    </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>253</v>
       </c>
@@ -12028,11 +11641,8 @@
       <c r="R208">
         <v>8992.1209699999999</v>
       </c>
-      <c r="S208">
-        <v>-0.44330083333333897</v>
-      </c>
-    </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>254</v>
       </c>
@@ -12087,11 +11697,8 @@
       <c r="R209">
         <v>9113.5932269999994</v>
       </c>
-      <c r="S209">
-        <v>-0.40578749999998798</v>
-      </c>
-    </row>
-    <row r="210" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>255</v>
       </c>
@@ -12146,11 +11753,8 @@
       <c r="R210">
         <v>9241.4633269999995</v>
       </c>
-      <c r="S210">
-        <v>-0.43371583333333702</v>
-      </c>
-    </row>
-    <row r="211" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>256</v>
       </c>
@@ -12205,11 +11809,8 @@
       <c r="R211">
         <v>9376.48514599999</v>
       </c>
-      <c r="S211">
-        <v>-0.53743249999999398</v>
-      </c>
-    </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>257</v>
       </c>
@@ -12264,11 +11865,8 @@
       <c r="R212">
         <v>9511.2070379999896</v>
       </c>
-      <c r="S212">
-        <v>-0.67576166666665904</v>
-      </c>
-    </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>258</v>
       </c>
@@ -12323,11 +11921,8 @@
       <c r="R213">
         <v>9667.9043450000008</v>
       </c>
-      <c r="S213">
-        <v>-0.144815833333339</v>
-      </c>
-    </row>
-    <row r="214" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>259</v>
       </c>
@@ -12382,11 +11977,8 @@
       <c r="R214">
         <v>9837.7982300000003</v>
       </c>
-      <c r="S214">
-        <v>-0.221549166666662</v>
-      </c>
-    </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>260</v>
       </c>
@@ -12441,11 +12033,8 @@
       <c r="R215">
         <v>10002.464250000001</v>
       </c>
-      <c r="S215">
-        <v>-5.8244999999999401E-2</v>
-      </c>
-    </row>
-    <row r="216" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>261</v>
       </c>
@@ -12500,11 +12089,8 @@
       <c r="R216">
         <v>10160.78751</v>
       </c>
-      <c r="S216">
-        <v>-0.87602916666666797</v>
-      </c>
-    </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>262</v>
       </c>
@@ -12559,11 +12145,8 @@
       <c r="R217">
         <v>10310.7019599999</v>
       </c>
-      <c r="S217">
-        <v>-1.84311000000001</v>
-      </c>
-    </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>263</v>
       </c>
@@ -12618,11 +12201,8 @@
       <c r="R218">
         <v>10469.673650000001</v>
       </c>
-      <c r="S218">
-        <v>-3.5500641666666701</v>
-      </c>
-    </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>264</v>
       </c>
@@ -12677,11 +12257,8 @@
       <c r="R219">
         <v>10618.901400000001</v>
       </c>
-      <c r="S219">
-        <v>-5.1644716666666701</v>
-      </c>
-    </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>265</v>
       </c>
@@ -12736,11 +12313,8 @@
       <c r="R220">
         <v>10742.049279999999</v>
       </c>
-      <c r="S220">
-        <v>-6.74364416666665</v>
-      </c>
-    </row>
-    <row r="221" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>266</v>
       </c>
@@ -12795,11 +12369,8 @@
       <c r="R221">
         <v>10852.96509</v>
       </c>
-      <c r="S221">
-        <v>-7.9103733333333199</v>
-      </c>
-    </row>
-    <row r="222" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>267</v>
       </c>
@@ -12854,11 +12425,8 @@
       <c r="R222">
         <v>10960.516659999999</v>
       </c>
-      <c r="S222">
-        <v>-7.65268999999999</v>
-      </c>
-    </row>
-    <row r="223" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>268</v>
       </c>
@@ -12913,11 +12481,8 @@
       <c r="R223">
         <v>11069.773999999999</v>
       </c>
-      <c r="S223">
-        <v>-6.6068483333333301</v>
-      </c>
-    </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>269</v>
       </c>
@@ -12972,11 +12537,8 @@
       <c r="R224">
         <v>11192.443229999901</v>
       </c>
-      <c r="S224">
-        <v>-6.0908658333333303</v>
-      </c>
-    </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>270</v>
       </c>
@@ -13031,11 +12593,8 @@
       <c r="R225">
         <v>11326.62543</v>
       </c>
-      <c r="S225">
-        <v>-5.9148858333333401</v>
-      </c>
-    </row>
-    <row r="226" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>271</v>
       </c>
@@ -13090,11 +12649,8 @@
       <c r="R226">
         <v>11451.72941</v>
       </c>
-      <c r="S226">
-        <v>-5.1988241666666601</v>
-      </c>
-    </row>
-    <row r="227" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>272</v>
       </c>
@@ -13149,11 +12705,8 @@
       <c r="R227">
         <v>11562.500539999999</v>
       </c>
-      <c r="S227">
-        <v>-5.5145024999999697</v>
-      </c>
-    </row>
-    <row r="228" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>273</v>
       </c>
@@ -13208,11 +12761,8 @@
       <c r="R228">
         <v>11699.594999999999</v>
       </c>
-      <c r="S228">
-        <v>-4.8360033333333297</v>
-      </c>
-    </row>
-    <row r="229" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>274</v>
       </c>
@@ -13267,11 +12817,8 @@
       <c r="R229">
         <v>11843.26613</v>
       </c>
-      <c r="S229">
-        <v>-3.9592608333333299</v>
-      </c>
-    </row>
-    <row r="230" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>275</v>
       </c>
@@ -13326,11 +12873,8 @@
       <c r="R230">
         <v>12002.115690000001</v>
       </c>
-      <c r="S230">
-        <v>-3.2790908333333202</v>
-      </c>
-    </row>
-    <row r="231" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>276</v>
       </c>
@@ -13385,11 +12929,8 @@
       <c r="R231">
         <v>12174.96017</v>
       </c>
-      <c r="S231">
-        <v>-2.6805366666666499</v>
-      </c>
-    </row>
-    <row r="232" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>277</v>
       </c>
@@ -13444,11 +12985,8 @@
       <c r="R232">
         <v>12330.283740000001</v>
       </c>
-      <c r="S232">
-        <v>-2.0913999999999899</v>
-      </c>
-    </row>
-    <row r="233" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>278</v>
       </c>
@@ -13503,11 +13041,8 @@
       <c r="R233">
         <v>12505.216259999999</v>
       </c>
-      <c r="S233">
-        <v>-0.92411833333332505</v>
-      </c>
-    </row>
-    <row r="234" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>279</v>
       </c>
@@ -13562,11 +13097,8 @@
       <c r="R234">
         <v>12683.22687</v>
       </c>
-      <c r="S234">
-        <v>0.13234249999999201</v>
-      </c>
-    </row>
-    <row r="235" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>280</v>
       </c>
@@ -13621,11 +13153,8 @@
       <c r="R235">
         <v>12850.620199999999</v>
       </c>
-      <c r="S235">
-        <v>0.39464749999998999</v>
-      </c>
-    </row>
-    <row r="236" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>281</v>
       </c>
@@ -13680,11 +13209,8 @@
       <c r="R236">
         <v>13042.589889999999</v>
       </c>
-      <c r="S236">
-        <v>-0.200717499999996</v>
-      </c>
-    </row>
-    <row r="237" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>282</v>
       </c>
@@ -13739,11 +13265,8 @@
       <c r="R237">
         <v>13223.02454</v>
       </c>
-      <c r="S237">
-        <v>0.23530499999999599</v>
-      </c>
-    </row>
-    <row r="238" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>283</v>
       </c>
@@ -13798,11 +13321,8 @@
       <c r="R238">
         <v>13387.825409999999</v>
       </c>
-      <c r="S238">
-        <v>0.68554250000001105</v>
-      </c>
-    </row>
-    <row r="239" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>284</v>
       </c>
@@ -13857,11 +13377,8 @@
       <c r="R239">
         <v>13574.2659199999</v>
       </c>
-      <c r="S239">
-        <v>0.82344833333331702</v>
-      </c>
-    </row>
-    <row r="240" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>285</v>
       </c>
@@ -13916,11 +13433,8 @@
       <c r="R240">
         <v>13735.82524</v>
       </c>
-      <c r="S240">
-        <v>0.75661333333334801</v>
-      </c>
-    </row>
-    <row r="241" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="241" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>286</v>
       </c>
@@ -13975,11 +13489,8 @@
       <c r="R241">
         <v>13848.42834</v>
       </c>
-      <c r="S241">
-        <v>0.49674333333334098</v>
-      </c>
-    </row>
-    <row r="242" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="242" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>287</v>
       </c>
@@ -14034,11 +13545,8 @@
       <c r="R242">
         <v>14045.73165</v>
       </c>
-      <c r="S242">
-        <v>0.851696666666654</v>
-      </c>
-    </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="243" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>288</v>
       </c>
@@ -14093,11 +13601,8 @@
       <c r="R243">
         <v>14212.10318</v>
       </c>
-      <c r="S243">
-        <v>1.40179916666667</v>
-      </c>
-    </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="244" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>289</v>
       </c>
@@ -14152,11 +13657,8 @@
       <c r="R244">
         <v>14361.15186</v>
       </c>
-      <c r="S244">
-        <v>1.3119049999999901</v>
-      </c>
-    </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="245" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>290</v>
       </c>
@@ -14211,11 +13713,8 @@
       <c r="R245">
         <v>14491.58066</v>
       </c>
-      <c r="S245">
-        <v>1.5605916666666599</v>
-      </c>
-    </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="246" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>291</v>
       </c>
@@ -14270,11 +13769,8 @@
       <c r="R246">
         <v>14618.168019999999</v>
       </c>
-      <c r="S246">
-        <v>1.44882500000001</v>
-      </c>
-    </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="247" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>292</v>
       </c>
@@ -14329,11 +13825,8 @@
       <c r="R247">
         <v>14761.03608</v>
       </c>
-      <c r="S247">
-        <v>0.398361666666673</v>
-      </c>
-    </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="248" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>293</v>
       </c>
@@ -14388,11 +13881,8 @@
       <c r="R248">
         <v>14942.714379999999</v>
       </c>
-      <c r="S248">
-        <v>-2.12883333333333</v>
-      </c>
-    </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="249" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>294</v>
       </c>
@@ -14447,11 +13937,8 @@
       <c r="R249">
         <v>15046.2381</v>
       </c>
-      <c r="S249">
-        <v>-5.4839849999999997</v>
-      </c>
-    </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="250" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>295</v>
       </c>
@@ -14506,11 +13993,8 @@
       <c r="R250">
         <v>15096.6798</v>
       </c>
-      <c r="S250">
-        <v>-9.5584516666666701</v>
-      </c>
-    </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="251" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>296</v>
       </c>
@@ -14565,11 +14049,8 @@
       <c r="R251">
         <v>15130.24626</v>
       </c>
-      <c r="S251">
-        <v>-11.28121</v>
-      </c>
-    </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="252" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>297</v>
       </c>
@@ -14624,11 +14105,8 @@
       <c r="R252">
         <v>15203.519689999999</v>
       </c>
-      <c r="S252">
-        <v>-9.8159524999999892</v>
-      </c>
-    </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="253" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>298</v>
       </c>
@@ -14683,11 +14161,8 @@
       <c r="R253">
         <v>15305.270699999999</v>
       </c>
-      <c r="S253">
-        <v>-8.0910066666666491</v>
-      </c>
-    </row>
-    <row r="254" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="254" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>299</v>
       </c>
@@ -14742,11 +14217,8 @@
       <c r="R254">
         <v>15403.516519999999</v>
       </c>
-      <c r="S254">
-        <v>-6.0259866666666602</v>
-      </c>
-    </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="255" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>300</v>
       </c>
@@ -14801,11 +14273,8 @@
       <c r="R255">
         <v>15533.996590000001</v>
       </c>
-      <c r="S255">
-        <v>-3.9980841666666498</v>
-      </c>
-    </row>
-    <row r="256" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="256" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>301</v>
       </c>
@@ -14860,11 +14329,8 @@
       <c r="R256">
         <v>15638.957419999901</v>
       </c>
-      <c r="S256">
-        <v>-2.4868233333333301</v>
-      </c>
-    </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="257" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>302</v>
       </c>
@@ -14919,11 +14385,8 @@
       <c r="R257">
         <v>15789.3742699999</v>
       </c>
-      <c r="S257">
-        <v>-1.7831791666666701</v>
-      </c>
-    </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="258" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>303</v>
       </c>
@@ -14978,11 +14441,8 @@
       <c r="R258">
         <v>15931.952219999999</v>
       </c>
-      <c r="S258">
-        <v>-1.1826191666666599</v>
-      </c>
-    </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="259" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>304</v>
       </c>
@@ -15037,11 +14497,8 @@
       <c r="R259">
         <v>16101.2166699999</v>
       </c>
-      <c r="S259">
-        <v>-0.887031666666658</v>
-      </c>
-    </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="260" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>305</v>
       </c>
@@ -15096,11 +14553,8 @@
       <c r="R260">
         <v>16264.438630000001</v>
       </c>
-      <c r="S260">
-        <v>-0.249489166666677</v>
-      </c>
-    </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="261" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>306</v>
       </c>
@@ -15155,11 +14609,8 @@
       <c r="R261">
         <v>16351.6132</v>
       </c>
-      <c r="S261">
-        <v>0.125794166666651</v>
-      </c>
-    </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="262" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>307</v>
       </c>
@@ -15214,11 +14665,8 @@
       <c r="R262">
         <v>16517.1281099999</v>
       </c>
-      <c r="S262">
-        <v>0.38917083333333802</v>
-      </c>
-    </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="263" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>308</v>
       </c>
@@ -15273,11 +14721,8 @@
       <c r="R263">
         <v>16657.125209999998</v>
       </c>
-      <c r="S263">
-        <v>0.38375999999999499</v>
-      </c>
-    </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="264" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>309</v>
       </c>
@@ -15332,11 +14777,8 @@
       <c r="R264">
         <v>16822.157350000001</v>
       </c>
-      <c r="S264">
-        <v>-8.1271666666665895E-2</v>
-      </c>
-    </row>
-    <row r="265" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="265" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>310</v>
       </c>
@@ -15391,11 +14833,8 @@
       <c r="R265">
         <v>16981.95275</v>
       </c>
-      <c r="S265">
-        <v>-0.127834166666659</v>
-      </c>
-    </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="266" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>311</v>
       </c>
@@ -15450,11 +14889,8 @@
       <c r="R266">
         <v>17126.82044</v>
       </c>
-      <c r="S266">
-        <v>9.0168333333337999E-2</v>
-      </c>
-    </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="267" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>312</v>
       </c>
@@ -15509,11 +14945,8 @@
       <c r="R267">
         <v>17242.403119999999</v>
       </c>
-      <c r="S267">
-        <v>0.13181749999999601</v>
-      </c>
-    </row>
-    <row r="268" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="268" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>313</v>
       </c>
@@ -15568,11 +15001,8 @@
       <c r="R268">
         <v>17406.678759999999</v>
       </c>
-      <c r="S268">
-        <v>0.202721666666661</v>
-      </c>
-    </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="269" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>314</v>
       </c>
@@ -15627,11 +15057,8 @@
       <c r="R269">
         <v>17580.204669999999</v>
       </c>
-      <c r="S269">
-        <v>0.51891416666666101</v>
-      </c>
-    </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="270" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>315</v>
       </c>
@@ -15686,11 +15113,8 @@
       <c r="R270">
         <v>17729.745340000001</v>
       </c>
-      <c r="S270">
-        <v>0.85072333333333405</v>
-      </c>
-    </row>
-    <row r="271" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="271" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>316</v>
       </c>
@@ -15745,11 +15169,8 @@
       <c r="R271">
         <v>17914.59679</v>
       </c>
-      <c r="S271">
-        <v>1.6907924999999999</v>
-      </c>
-    </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="272" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>317</v>
       </c>
@@ -15804,11 +15225,8 @@
       <c r="R272">
         <v>18074.92195</v>
       </c>
-      <c r="S272">
-        <v>1.8846341666666699</v>
-      </c>
-    </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="273" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>318</v>
       </c>
@@ -15863,11 +15281,8 @@
       <c r="R273">
         <v>18181.00086</v>
       </c>
-      <c r="S273">
-        <v>2.1338224999999902</v>
-      </c>
-    </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="274" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>319</v>
       </c>
@@ -15922,11 +15337,8 @@
       <c r="R274">
         <v>18260.110290000001</v>
       </c>
-      <c r="S274">
-        <v>1.19472166666668</v>
-      </c>
-    </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="275" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>320</v>
       </c>
@@ -15981,11 +15393,8 @@
       <c r="R275">
         <v>18455.77965</v>
       </c>
-      <c r="S275">
-        <v>0.19019583333333401</v>
-      </c>
-    </row>
-    <row r="276" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="276" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>321</v>
       </c>
@@ -16040,11 +15449,8 @@
       <c r="R276">
         <v>18596.21773</v>
       </c>
-      <c r="S276">
-        <v>0.361814999999992</v>
-      </c>
-    </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="277" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>322</v>
       </c>
@@ -16099,11 +15505,8 @@
       <c r="R277">
         <v>18687.608230000002</v>
       </c>
-      <c r="S277">
-        <v>-0.53896749999999805</v>
-      </c>
-    </row>
-    <row r="278" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="278" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>323</v>
       </c>
@@ -16158,11 +15561,8 @@
       <c r="R278">
         <v>18763.324339999999</v>
       </c>
-      <c r="S278">
-        <v>-0.88720750000000204</v>
-      </c>
-    </row>
-    <row r="279" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="279" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>324</v>
       </c>
@@ -16217,11 +15617,8 @@
       <c r="R279">
         <v>18983.64286</v>
       </c>
-      <c r="S279">
-        <v>-1.04759583333333</v>
-      </c>
-    </row>
-    <row r="280" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="280" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>325</v>
       </c>
@@ -16276,11 +15673,8 @@
       <c r="R280">
         <v>19125.0067099999</v>
       </c>
-      <c r="S280">
-        <v>-0.85218666666666798</v>
-      </c>
-    </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="281" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>326</v>
       </c>
@@ -16335,11 +15729,8 @@
       <c r="R281">
         <v>19310.567069999899</v>
       </c>
-      <c r="S281">
-        <v>-0.94214333333334799</v>
-      </c>
-    </row>
-    <row r="282" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="282" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>327</v>
       </c>
@@ -16394,11 +15785,8 @@
       <c r="R282">
         <v>19502.60772</v>
       </c>
-      <c r="S282">
-        <v>-0.83311166666666703</v>
-      </c>
-    </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="283" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>328</v>
       </c>
@@ -16453,11 +15841,8 @@
       <c r="R283">
         <v>19648.047930000001</v>
       </c>
-      <c r="S283">
-        <v>0.47224583333333198</v>
-      </c>
-    </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="284" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>329</v>
       </c>
@@ -16512,11 +15897,8 @@
       <c r="R284">
         <v>19846.550209999899</v>
       </c>
-      <c r="S284">
-        <v>0.52975583333333898</v>
-      </c>
-    </row>
-    <row r="285" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="285" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>330</v>
       </c>
@@ -16571,11 +15953,8 @@
       <c r="R285">
         <v>20069.215560000001</v>
       </c>
-      <c r="S285">
-        <v>1.8948716666666501</v>
-      </c>
-    </row>
-    <row r="286" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="286" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>331</v>
       </c>
@@ -16630,11 +16009,8 @@
       <c r="R286">
         <v>20300.652030000001</v>
       </c>
-      <c r="S286">
-        <v>2.5496958333333302</v>
-      </c>
-    </row>
-    <row r="287" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="287" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>332</v>
       </c>
@@ -16689,11 +16065,8 @@
       <c r="R287">
         <v>20551.45563</v>
       </c>
-      <c r="S287">
-        <v>3.5392316666666499</v>
-      </c>
-    </row>
-    <row r="288" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="288" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>333</v>
       </c>
@@ -16748,11 +16121,8 @@
       <c r="R288">
         <v>20749.390950000001</v>
       </c>
-      <c r="S288">
-        <v>4.0544049999999796</v>
-      </c>
-    </row>
-    <row r="289" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="289" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>334</v>
       </c>
@@ -16807,11 +16177,8 @@
       <c r="R289">
         <v>20949.010419999999</v>
       </c>
-      <c r="S289">
-        <v>3.8773825000000102</v>
-      </c>
-    </row>
-    <row r="290" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="290" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>335</v>
       </c>
@@ -16866,11 +16233,8 @@
       <c r="R290">
         <v>21123.413550000001</v>
       </c>
-      <c r="S290">
-        <v>2.62001666666665</v>
-      </c>
-    </row>
-    <row r="291" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="291" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>336</v>
       </c>
@@ -16925,11 +16289,8 @@
       <c r="R291">
         <v>21344.738310000001</v>
       </c>
-      <c r="S291">
-        <v>1.5807024999999999</v>
-      </c>
-    </row>
-    <row r="292" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="292" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>337</v>
       </c>
@@ -16984,11 +16345,8 @@
       <c r="R292">
         <v>21525.169300000001</v>
       </c>
-      <c r="S292">
-        <v>1.04900833333333</v>
-      </c>
-    </row>
-    <row r="293" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="293" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>338</v>
       </c>
@@ -17043,11 +16401,8 @@
       <c r="R293">
         <v>21701.77879</v>
       </c>
-      <c r="S293">
-        <v>0.238385833333325</v>
-      </c>
-    </row>
-    <row r="294" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="294" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>339</v>
       </c>
@@ -17102,11 +16457,8 @@
       <c r="R294">
         <v>21910.4794</v>
       </c>
-      <c r="S294">
-        <v>-1.2461916666666599</v>
-      </c>
-    </row>
-    <row r="295" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="295" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>340</v>
       </c>
@@ -17161,11 +16513,8 @@
       <c r="R295">
         <v>21937.478340000001</v>
       </c>
-      <c r="S295">
-        <v>-10.507066666666599</v>
-      </c>
-    </row>
-    <row r="296" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="296" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>341</v>
       </c>
@@ -17220,11 +16569,8 @@
       <c r="R296">
         <v>22236.468499999999</v>
       </c>
-      <c r="S296">
-        <v>-3.9408150000000002</v>
-      </c>
-    </row>
-    <row r="297" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="297" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>342</v>
       </c>
@@ -17279,11 +16625,8 @@
       <c r="R297">
         <v>22496.5728099999</v>
       </c>
-      <c r="S297">
-        <v>-2.21587916666665</v>
-      </c>
-    </row>
-    <row r="298" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="298" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>343</v>
       </c>
@@ -17338,11 +16681,8 @@
       <c r="R298">
         <v>22892.748960000001</v>
       </c>
-      <c r="S298">
-        <v>-1.59363083333332</v>
-      </c>
-    </row>
-    <row r="299" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="299" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>344</v>
       </c>
@@ -17397,11 +16737,8 @@
       <c r="R299">
         <v>23362.233550000001</v>
       </c>
-      <c r="S299">
-        <v>5.5654999999987298E-2</v>
-      </c>
-    </row>
-    <row r="300" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="300" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>345</v>
       </c>
@@ -17456,11 +16793,8 @@
       <c r="R300">
         <v>23835.078109999999</v>
       </c>
-      <c r="S300">
-        <v>0.70337083333332295</v>
-      </c>
-    </row>
-    <row r="301" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="301" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>346</v>
       </c>
@@ -17515,11 +16849,8 @@
       <c r="R301">
         <v>24377.236430000001</v>
       </c>
-      <c r="S301">
-        <v>1.4992175000000001</v>
-      </c>
-    </row>
-    <row r="302" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="302" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>347</v>
       </c>
@@ -17574,11 +16905,8 @@
       <c r="R302">
         <v>25006.127509999998</v>
       </c>
-      <c r="S302">
-        <v>1.7227249999999801</v>
-      </c>
-    </row>
-    <row r="303" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="303" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>348</v>
       </c>
@@ -17633,11 +16961,8 @@
       <c r="R303">
         <v>25713.223440000002</v>
       </c>
-      <c r="S303">
-        <v>1.98078166666667</v>
-      </c>
-    </row>
-    <row r="304" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="304" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>349</v>
       </c>
@@ -17692,11 +17017,8 @@
       <c r="R304">
         <v>26146.675080000001</v>
       </c>
-      <c r="S304">
-        <v>1.6952225000000101</v>
-      </c>
-    </row>
-    <row r="305" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="305" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>350</v>
       </c>
@@ -17751,11 +17073,8 @@
       <c r="R305">
         <v>26536.55228</v>
       </c>
-      <c r="S305">
-        <v>0.96557333333332396</v>
-      </c>
-    </row>
-    <row r="306" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="306" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>351</v>
       </c>
@@ -17810,11 +17129,8 @@
       <c r="R306">
         <v>26927.76916</v>
       </c>
-      <c r="S306">
-        <v>0.69529166666666198</v>
-      </c>
-    </row>
-    <row r="307" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="307" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>352</v>
       </c>
@@ -17869,16 +17185,13 @@
       <c r="R307">
         <v>27202.53426</v>
       </c>
-      <c r="S307">
-        <v>0.44353833333332199</v>
-      </c>
-    </row>
-    <row r="308" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="308" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M308" s="7"/>
       <c r="N308" s="5"/>
       <c r="O308" s="5"/>
     </row>
-    <row r="309" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N309" s="5"/>
       <c r="O309" s="5"/>
     </row>
@@ -17889,10 +17202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A502E475-8EEE-9B41-8582-BA225638D4DC}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18113,14 +17426,6 @@
       </c>
       <c r="C21" s="3" t="s">
         <v>364</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>368</v>
-      </c>
-      <c r="B22" t="s">
-        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>